<commit_message>
Forms. Just quick notes for the form line
</commit_message>
<xml_diff>
--- a/src/pages/_Note_AddAdPage.jsx.xlsx
+++ b/src/pages/_Note_AddAdPage.jsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\deivi\Documents\deividas_vaitkus_type1_galutine_praktine_uzduotis_front\src\pages\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C571C6D-262D-46D2-960F-0DDE4E42751A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5C828D-8700-49B8-9687-8E47814E20F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11052" yWindow="2556" windowWidth="17280" windowHeight="8880" xr2:uid="{A9C9D30F-8E1A-480D-8E91-CF67A981FDCD}"/>
+    <workbookView xWindow="3276" yWindow="2052" windowWidth="17280" windowHeight="8880" xr2:uid="{A9C9D30F-8E1A-480D-8E91-CF67A981FDCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>Margin</t>
   </si>
@@ -43,6 +43,21 @@
   </si>
   <si>
     <t>Sum</t>
+  </si>
+  <si>
+    <t>PC view</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> #1. The lines with two inputs</t>
+  </si>
+  <si>
+    <t>The lines with one input</t>
   </si>
 </sst>
 </file>
@@ -84,7 +99,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -166,7 +181,7 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
@@ -184,6 +199,19 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -196,36 +224,161 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top style="hair">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,128 +693,210 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F45D703-3B76-4275-8E7E-9EF17EFD3810}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="0.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="1.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="8"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="5" t="s">
+    <row r="1" spans="1:10" ht="1.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="7"/>
+      <c r="B3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="17"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="11">
+        <v>0.25</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="14"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="3">
+        <v>0.25</v>
+      </c>
+      <c r="I4" s="20">
+        <f>SUM(C4:H4)</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="7"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="7"/>
+      <c r="B5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="F5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I5" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="8"/>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="J5" s="7"/>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="11">
         <v>0.25</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D6" s="12"/>
+      <c r="E6" s="2">
         <v>0.125</v>
       </c>
-      <c r="E3" s="3">
+      <c r="F6" s="2">
         <v>0.125</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G6" s="2">
         <v>0.25</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H6" s="3">
         <v>0.25</v>
       </c>
-      <c r="H3" s="1">
-        <f>SUM(B3:G3)</f>
+      <c r="I6" s="1">
+        <f>SUM(C6:H6)</f>
         <v>1</v>
       </c>
-      <c r="I3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="8"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="8"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="9"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="8"/>
-      <c r="I8" s="8"/>
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="7"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="7"/>
     </row>
   </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C2:I2"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E3:G3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>